<commit_message>
Fixed bug in get_F ran lin heur one group 90 days
</commit_message>
<xml_diff>
--- a/benchmarks/all_results_one_group.xlsx
+++ b/benchmarks/all_results_one_group.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergioacamelogomez/Dropbox/covid-optimization/benchmarks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/afs/ir.stanford.edu/users/x/w/xwarnes/GitHub/covid-optimization/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D4E602-AA65-5E4B-BD60-0644DBDCAEF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F5875D-2C23-C14B-A6F1-16104F23E9D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-580" yWindow="3000" windowWidth="21000" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$37</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
   <si>
     <t>heuristic</t>
   </si>
@@ -68,13 +71,25 @@
   </si>
   <si>
     <t>eta</t>
+  </si>
+  <si>
+    <t>linearization_heuristic</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing</t>
+  </si>
+  <si>
+    <t>lockdown_freq</t>
+  </si>
+  <si>
+    <t>test_freq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +104,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -145,6 +165,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O21"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -530,17 +559,19 @@
       <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="L1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -554,28 +585,29 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
       <c r="H2">
-        <v>33922389065.674919</v>
+        <v>52678430562.986076</v>
       </c>
       <c r="I2">
-        <v>10735.6693187202</v>
+        <v>1.3950503911198271</v>
       </c>
       <c r="J2">
-        <v>30380279979.137051</v>
+        <v>48075624235.906647</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -589,28 +621,29 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
       <c r="H3">
-        <v>26957238971.678761</v>
+        <v>52678430562.986076</v>
       </c>
       <c r="I3">
-        <v>9754.2051025157343</v>
+        <v>1.395050391119828</v>
       </c>
       <c r="J3">
-        <v>23738952575.195919</v>
+        <v>48075624235.906647</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -624,34 +657,35 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
       <c r="H4">
-        <v>47123039801.550148</v>
+        <v>52863133977.572906</v>
       </c>
       <c r="I4">
-        <v>72870.419798581148</v>
+        <v>14684.8789984668</v>
       </c>
       <c r="J4">
-        <v>23080293285.662289</v>
+        <v>48018029141.447121</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="L4">
+        <v>14</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>0.5</v>
       </c>
       <c r="D5">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>3000</v>
@@ -659,34 +693,37 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
       <c r="H5">
-        <v>33922389065.674919</v>
+        <v>52863133977.572906</v>
       </c>
       <c r="I5">
-        <v>10735.6693187202</v>
+        <v>1.4684878998466819</v>
       </c>
       <c r="J5">
-        <v>19644610660.416851</v>
+        <v>48018029141.447121</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="L5">
+        <v>14</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>0.5</v>
       </c>
       <c r="D6">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>3000</v>
@@ -698,30 +735,30 @@
         <v>9</v>
       </c>
       <c r="H6">
-        <v>26957238971.678761</v>
+        <v>52715376635.427467</v>
       </c>
       <c r="I6">
-        <v>9754.2051025157343</v>
+        <v>15317.425248107909</v>
       </c>
       <c r="J6">
-        <v>13984747472.680201</v>
+        <v>47661570529.544594</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>0.5</v>
       </c>
       <c r="D7">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>3000</v>
@@ -733,24 +770,22 @@
         <v>9</v>
       </c>
       <c r="H7">
-        <v>47123039801.550148</v>
+        <v>50746103565.542236</v>
       </c>
       <c r="I7">
-        <v>72870.419798581148</v>
+        <v>17643.318105167731</v>
       </c>
       <c r="J7">
-        <v>-49790126512.918861</v>
+        <v>44924896193.960968</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>0</v>
-      </c>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>0.5</v>
@@ -764,34 +799,35 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
       <c r="H8">
-        <v>45878900163.079453</v>
+        <v>46283013883.96788</v>
       </c>
       <c r="I8">
-        <v>14226.336224976299</v>
+        <v>1.0835556427290931</v>
       </c>
       <c r="J8">
-        <v>41185086175.835777</v>
+        <v>42707948209.033638</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>0.5</v>
       </c>
       <c r="D9">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>3000</v>
@@ -799,90 +835,95 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
       <c r="H9">
-        <v>44283791622.124352</v>
+        <v>46283013883.96788</v>
       </c>
       <c r="I9">
-        <v>11550.173796724799</v>
+        <v>1.0835556427290931</v>
       </c>
       <c r="J9">
-        <v>28922772470.36137</v>
+        <v>42707948209.033638</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>3000</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>46505839470.089653</v>
+      </c>
+      <c r="I10">
+        <v>11641.193385054799</v>
+      </c>
+      <c r="J10">
+        <v>42664963261.70594</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>14</v>
       </c>
-      <c r="C10">
-        <v>0.5</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>3000</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>46354898378.35994</v>
-      </c>
-      <c r="I10">
-        <v>12490.37457217191</v>
-      </c>
-      <c r="J10">
-        <v>42233844725.076797</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
+      <c r="M10">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>3000</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>46505839470.089653</v>
+      </c>
+      <c r="I11">
+        <v>11641.193385054799</v>
+      </c>
+      <c r="J11">
+        <v>42664963261.70594</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>14</v>
       </c>
-      <c r="C11">
-        <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>1000000</v>
-      </c>
-      <c r="E11">
-        <v>3000</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11">
-        <v>42636603549.971458</v>
-      </c>
-      <c r="I11">
-        <v>6505.0261501660134</v>
-      </c>
-      <c r="J11">
-        <v>33985319765.501148</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
+      <c r="M11">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -890,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>0.5</v>
@@ -908,24 +949,24 @@
         <v>9</v>
       </c>
       <c r="H12">
-        <v>39077163200.547081</v>
+        <v>46354898378.35994</v>
       </c>
       <c r="I12">
-        <v>10735.6693187202</v>
+        <v>12490.37457217191</v>
       </c>
       <c r="J12">
-        <v>35535054114.009209</v>
+        <v>42233844725.076797</v>
       </c>
       <c r="K12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>0.5</v>
@@ -943,30 +984,28 @@
         <v>9</v>
       </c>
       <c r="H13">
-        <v>31455932197.26899</v>
+        <v>45878900163.079453</v>
       </c>
       <c r="I13">
-        <v>9754.2051025157343</v>
+        <v>14226.336224976299</v>
       </c>
       <c r="J13">
-        <v>28237645800.78616</v>
+        <v>41185086175.835777</v>
       </c>
       <c r="K13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>0.5</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="E14">
         <v>3000</v>
@@ -974,28 +1013,29 @@
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
       <c r="H14">
-        <v>60653085932.746803</v>
+        <v>48453689270.580833</v>
       </c>
       <c r="I14">
-        <v>72870.419798581148</v>
+        <v>6399.6249983453499</v>
       </c>
       <c r="J14">
-        <v>36610339416.858963</v>
+        <v>39942582520.692833</v>
       </c>
       <c r="K14">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>3</v>
-      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>0.5</v>
@@ -1009,28 +1049,29 @@
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
       <c r="H15">
-        <v>39077163200.547081</v>
+        <v>48453689270.580833</v>
       </c>
       <c r="I15">
-        <v>10735.6693187202</v>
+        <v>6399.6249983453499</v>
       </c>
       <c r="J15">
-        <v>24799384795.28899</v>
+        <v>39942582520.692833</v>
       </c>
       <c r="K15">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>4</v>
-      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0.5</v>
@@ -1044,28 +1085,29 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
       <c r="H16">
-        <v>31455932197.26899</v>
+        <v>48760641602.50148</v>
       </c>
       <c r="I16">
-        <v>9754.2051025157343</v>
+        <v>6833.7924808001899</v>
       </c>
       <c r="J16">
-        <v>18483440698.27042</v>
+        <v>39672118864.730026</v>
       </c>
       <c r="K16">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>5</v>
-      </c>
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="M16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0.5</v>
@@ -1079,34 +1121,37 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
       <c r="H17">
-        <v>60653085932.746803</v>
+        <v>48760641602.50148</v>
       </c>
       <c r="I17">
-        <v>72870.419798581148</v>
+        <v>6833.7924808001899</v>
       </c>
       <c r="J17">
-        <v>-36260080381.722153</v>
+        <v>39672118864.730026</v>
       </c>
       <c r="K17">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>14</v>
+      </c>
+      <c r="M17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>0.5</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="E18">
         <v>3000</v>
@@ -1118,30 +1163,30 @@
         <v>9</v>
       </c>
       <c r="H18">
-        <v>50746103565.542236</v>
+        <v>47758769889.649063</v>
       </c>
       <c r="I18">
-        <v>17643.318105167731</v>
+        <v>6572.3037463550099</v>
       </c>
       <c r="J18">
-        <v>44924896193.960968</v>
+        <v>39018011049.501534</v>
       </c>
       <c r="K18">
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>0.5</v>
       </c>
       <c r="D19">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>3000</v>
@@ -1153,24 +1198,24 @@
         <v>9</v>
       </c>
       <c r="H19">
-        <v>45650382877.360222</v>
+        <v>60653085932.746803</v>
       </c>
       <c r="I19">
-        <v>11870.15677305763</v>
+        <v>72870.419798581148</v>
       </c>
       <c r="J19">
-        <v>29863806092.07658</v>
+        <v>36610339416.858963</v>
       </c>
       <c r="K19">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>0.5</v>
@@ -1188,24 +1233,22 @@
         <v>9</v>
       </c>
       <c r="H20">
-        <v>52715376635.427467</v>
+        <v>39077163200.547081</v>
       </c>
       <c r="I20">
-        <v>15317.425248107909</v>
+        <v>10735.6693187202</v>
       </c>
       <c r="J20">
-        <v>47661570529.544594</v>
+        <v>35535054114.009209</v>
       </c>
       <c r="K20">
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>0.5</v>
@@ -1219,24 +1262,598 @@
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21" t="s">
-        <v>9</v>
-      </c>
       <c r="H21">
-        <v>47758769889.649063</v>
+        <v>43137204794.196877</v>
       </c>
       <c r="I21">
-        <v>6572.3037463550099</v>
+        <v>0.61696495472009716</v>
       </c>
       <c r="J21">
-        <v>39018011049.501534</v>
+        <v>34931951217.744743</v>
       </c>
       <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>1000000</v>
+      </c>
+      <c r="E22">
+        <v>3000</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>43137204794.196877</v>
+      </c>
+      <c r="I22">
+        <v>0.61696495472009716</v>
+      </c>
+      <c r="J22">
+        <v>34931951217.744743</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>1000000</v>
+      </c>
+      <c r="E23">
+        <v>3000</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>43189201116.213783</v>
+      </c>
+      <c r="I23">
+        <v>6410.1138590013597</v>
+      </c>
+      <c r="J23">
+        <v>34664144828.227676</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>14</v>
+      </c>
+      <c r="M23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <v>1000000</v>
+      </c>
+      <c r="E24">
+        <v>3000</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>43189201116.213783</v>
+      </c>
+      <c r="I24">
+        <v>6410.1138590013597</v>
+      </c>
+      <c r="J24">
+        <v>34664144828.227676</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>14</v>
+      </c>
+      <c r="M24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25">
+        <v>1000000</v>
+      </c>
+      <c r="E25">
+        <v>3000</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25">
+        <v>42636603549.971458</v>
+      </c>
+      <c r="I25">
+        <v>6505.0261501660134</v>
+      </c>
+      <c r="J25">
+        <v>33985319765.501148</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>3000</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>33922389065.674919</v>
+      </c>
+      <c r="I26">
+        <v>10735.6693187202</v>
+      </c>
+      <c r="J26">
+        <v>30380279979.137051</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>1000000</v>
+      </c>
+      <c r="E27">
+        <v>3000</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>45650382877.360222</v>
+      </c>
+      <c r="I27">
+        <v>11870.15677305763</v>
+      </c>
+      <c r="J27">
+        <v>29863806092.07658</v>
+      </c>
+      <c r="K27">
         <v>0.1</v>
       </c>
     </row>
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>1000000</v>
+      </c>
+      <c r="E28">
+        <v>3000</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <v>44283791622.124352</v>
+      </c>
+      <c r="I28">
+        <v>11550.173796724799</v>
+      </c>
+      <c r="J28">
+        <v>28922772470.36137</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>3000</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29">
+        <v>31455932197.26899</v>
+      </c>
+      <c r="I29">
+        <v>9754.2051025157343</v>
+      </c>
+      <c r="J29">
+        <v>28237645800.78616</v>
+      </c>
+      <c r="K29">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30">
+        <v>1000000</v>
+      </c>
+      <c r="E30">
+        <v>3000</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <v>39077163200.547081</v>
+      </c>
+      <c r="I30">
+        <v>10735.6693187202</v>
+      </c>
+      <c r="J30">
+        <v>24799384795.28899</v>
+      </c>
+      <c r="K30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>3000</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>26957238971.678761</v>
+      </c>
+      <c r="I31">
+        <v>9754.2051025157343</v>
+      </c>
+      <c r="J31">
+        <v>23738952575.195919</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>3000</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32">
+        <v>47123039801.550148</v>
+      </c>
+      <c r="I32">
+        <v>72870.419798581148</v>
+      </c>
+      <c r="J32">
+        <v>23080293285.662289</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>0.5</v>
+      </c>
+      <c r="D33">
+        <v>1000000</v>
+      </c>
+      <c r="E33">
+        <v>3000</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>33922389065.674919</v>
+      </c>
+      <c r="I33">
+        <v>10735.6693187202</v>
+      </c>
+      <c r="J33">
+        <v>19644610660.416851</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34">
+        <v>1000000</v>
+      </c>
+      <c r="E34">
+        <v>3000</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>31455932197.26899</v>
+      </c>
+      <c r="I34">
+        <v>9754.2051025157343</v>
+      </c>
+      <c r="J34">
+        <v>18483440698.27042</v>
+      </c>
+      <c r="K34">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>0.5</v>
+      </c>
+      <c r="D35">
+        <v>1000000</v>
+      </c>
+      <c r="E35">
+        <v>3000</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>26957238971.678761</v>
+      </c>
+      <c r="I35">
+        <v>9754.2051025157343</v>
+      </c>
+      <c r="J35">
+        <v>13984747472.680201</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36">
+        <v>1000000</v>
+      </c>
+      <c r="E36">
+        <v>3000</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36">
+        <v>60653085932.746803</v>
+      </c>
+      <c r="I36">
+        <v>72870.419798581148</v>
+      </c>
+      <c r="J36">
+        <v>-36260080381.722153</v>
+      </c>
+      <c r="K36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>0.5</v>
+      </c>
+      <c r="D37">
+        <v>1000000</v>
+      </c>
+      <c r="E37">
+        <v>3000</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>47123039801.550148</v>
+      </c>
+      <c r="I37">
+        <v>72870.419798581148</v>
+      </c>
+      <c r="J37">
+        <v>-49790126512.918861</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O9">
+  <autoFilter ref="A1:M37" xr:uid="{E6C3897B-5723-8442-B578-07361D83BF2E}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:M37">
+      <sortCondition descending="1" ref="J1:J37"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:O9">
     <sortCondition ref="J2:J9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added runs of lin
</commit_message>
<xml_diff>
--- a/benchmarks/all_results_one_group.xlsx
+++ b/benchmarks/all_results_one_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/afs/ir.stanford.edu/users/x/w/xwarnes/GitHub/covid-optimization/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F5875D-2C23-C14B-A6F1-16104F23E9D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A1F3F1-08CF-E64F-9970-FA252DF9557D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-580" yWindow="3000" windowWidth="21000" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="14320" windowWidth="21000" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,16 +511,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
     <col min="10" max="10" width="9.83203125" customWidth="1"/>
@@ -996,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>16</v>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>17</v>
@@ -1068,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>16</v>
@@ -1104,7 +1104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>17</v>
@@ -1140,7 +1140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>16</v>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" t="s">
         <v>17</v>
@@ -1317,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>1</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>1</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>1</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>3</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>3</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>4</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>4</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>5</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>5</v>
       </c>
@@ -1843,16 +1843,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M37" xr:uid="{E6C3897B-5723-8442-B578-07361D83BF2E}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="0"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:M37">
-      <sortCondition descending="1" ref="J1:J37"/>
-    </sortState>
-  </autoFilter>
   <sortState ref="A2:O9">
     <sortCondition ref="J2:J9"/>
   </sortState>

</xml_diff>